<commit_message>
Create facebook friend search test case
</commit_message>
<xml_diff>
--- a/ejemplos_clase/Facebook_Friend_Search_Scenario.xlsx
+++ b/ejemplos_clase/Facebook_Friend_Search_Scenario.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="23055" windowHeight="10320"/>
+    <workbookView xWindow="1890" yWindow="0" windowWidth="23055" windowHeight="10320"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -51,46 +51,79 @@
     <t>Buscar a un amigo en facebook</t>
   </si>
   <si>
-    <t>- Facebook esta arriba
-- La persona a buscar tiene que estar registrado en facebook</t>
-  </si>
-  <si>
-    <t>Exploradores:
-- Iexplorer
--Firefox
-- chrome
-- safari</t>
-  </si>
-  <si>
     <t>Ingresar el nombre de la persona a buscar en el campo buscar</t>
-  </si>
-  <si>
-    <t>El nombre es ingresado correctamente en el campo</t>
-  </si>
-  <si>
-    <t>Lidia sandrose</t>
   </si>
   <si>
     <t>Presionar la tecla enter</t>
   </si>
   <si>
-    <t>Facebook redirigira la pagina al perfil de la persona</t>
+    <t>- La pagina facebook.com esta disponible
+- La persona a buscar ya esta registrada en facebook</t>
   </si>
   <si>
-    <t>facebook abre correctamente en el navegador</t>
+    <t>Ingresar la URL en el navegador</t>
   </si>
   <si>
-    <t>1. facebook.com</t>
+    <t xml:space="preserve">Chrome
+</t>
   </si>
   <si>
-    <t>Ingresar usuario y contrase</t>
+    <t>El navegador abre correctamente</t>
+  </si>
+  <si>
+    <t>La URL es ingresada correctamente</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com</t>
+  </si>
+  <si>
+    <t>La pagina facebook.com es mostrada correctamente</t>
+  </si>
+  <si>
+    <t>Ingresar correo electronico</t>
+  </si>
+  <si>
+    <t>El correo electronico es ingresado correctamente</t>
+  </si>
+  <si>
+    <t>ivonne_852@hotmail.com</t>
+  </si>
+  <si>
+    <t>Ingresar contraseña</t>
+  </si>
+  <si>
+    <t>La contraseña se ha ingresado correctamente</t>
+  </si>
+  <si>
+    <t>******</t>
+  </si>
+  <si>
+    <t>Click en el boton entrar</t>
+  </si>
+  <si>
+    <t>La pagina principal del perfil es cargada correctamente</t>
+  </si>
+  <si>
+    <t>Juan Perez</t>
+  </si>
+  <si>
+    <t>El nombre es ingresado correctamente en el campo y se mostrara automaticamente una lista de posibles perfiles que correspondan al nombre ingresado</t>
+  </si>
+  <si>
+    <t>Facebook mostrara la lista mas detallada de posibles perfiles que correspondan al nombre ingresado</t>
+  </si>
+  <si>
+    <t>Seleccionar el perfil de Juan Perez</t>
+  </si>
+  <si>
+    <t>Asegurar que el perfil de Juan Perez sea el correcto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -104,6 +137,12 @@
     <font>
       <sz val="11"/>
       <name val="Ubuntu"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -136,10 +175,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -161,8 +201,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -441,17 +485,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1002"/>
+  <dimension ref="A1:G1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
@@ -474,7 +518,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="45" customHeight="1">
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -482,7 +526,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -535,7 +579,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="75">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="7">
         <v>1</v>
       </c>
@@ -543,127 +587,157 @@
         <v>8</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="D7" s="8"/>
       <c r="E7" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" s="2" customFormat="1" ht="28.5">
-      <c r="A8" s="7"/>
+      <c r="A8" s="7">
+        <v>2</v>
+      </c>
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="8"/>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="75" customHeight="1">
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="28.5">
       <c r="A9" s="7">
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>13</v>
+      <c r="C9" s="6" t="s">
+        <v>18</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1">
+      <c r="D9" s="8"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="28.5">
       <c r="A10" s="7">
         <v>3</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>15</v>
+      <c r="B10" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
+      <c r="D10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1">
+      <c r="A11" s="7">
+        <v>4</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="28.5">
+      <c r="A12" s="7">
+        <v>5</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" ht="75" customHeight="1">
+      <c r="A13" s="7">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="E13" s="7"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
+    <row r="14" spans="1:7" ht="30" customHeight="1">
+      <c r="A14" s="7">
+        <v>7</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="6"/>
       <c r="E14" s="7"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+    <row r="15" spans="1:7" ht="30" customHeight="1">
+      <c r="A15" s="7">
+        <v>8</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
@@ -9523,7 +9597,47 @@
       <c r="F1002" s="2"/>
       <c r="G1002" s="2"/>
     </row>
+    <row r="1003" spans="1:7">
+      <c r="A1003" s="2"/>
+      <c r="B1003" s="2"/>
+      <c r="C1003" s="2"/>
+      <c r="D1003" s="2"/>
+      <c r="E1003" s="2"/>
+      <c r="F1003" s="2"/>
+      <c r="G1003" s="2"/>
+    </row>
+    <row r="1004" spans="1:7">
+      <c r="A1004" s="2"/>
+      <c r="B1004" s="2"/>
+      <c r="C1004" s="2"/>
+      <c r="D1004" s="2"/>
+      <c r="E1004" s="2"/>
+      <c r="F1004" s="2"/>
+      <c r="G1004" s="2"/>
+    </row>
+    <row r="1005" spans="1:7">
+      <c r="A1005" s="2"/>
+      <c r="B1005" s="2"/>
+      <c r="C1005" s="2"/>
+      <c r="D1005" s="2"/>
+      <c r="E1005" s="2"/>
+      <c r="F1005" s="2"/>
+      <c r="G1005" s="2"/>
+    </row>
+    <row r="1006" spans="1:7">
+      <c r="A1006" s="2"/>
+      <c r="B1006" s="2"/>
+      <c r="C1006" s="2"/>
+      <c r="D1006" s="2"/>
+      <c r="E1006" s="2"/>
+      <c r="F1006" s="2"/>
+      <c r="G1006" s="2"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D8" r:id="rId1"/>
+    <hyperlink ref="D10" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>